<commit_message>
9th April status updated
</commit_message>
<xml_diff>
--- a/Daily Status update Report 08-04-2020.xlsx
+++ b/Daily Status update Report 08-04-2020.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="142">
   <si>
     <t>Sr.No</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>Discussion on SLA document for PT; Working on cucumber</t>
+  </si>
+  <si>
+    <t>Keyword Driven Framework Completed ;</t>
   </si>
 </sst>
 </file>
@@ -7497,7 +7500,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7785,7 +7790,9 @@
       <c r="F13" s="38">
         <v>0.75</v>
       </c>
-      <c r="G13" s="36"/>
+      <c r="G13" s="36" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="35">

</xml_diff>

<commit_message>
Updated status for 9th April - Pratiksha and Me
</commit_message>
<xml_diff>
--- a/Daily Status update Report 08-04-2020.xlsx
+++ b/Daily Status update Report 08-04-2020.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="143">
   <si>
     <t>Sr.No</t>
   </si>
@@ -451,12 +451,18 @@
   <si>
     <t>Discussion on SLA document for PT; Working on cucumber</t>
   </si>
+  <si>
+    <t>Completed with Test Cases Writing for Collateral Withdraw Cash - Checked-Checked-Margin Deposit Scenario(for Created-&gt;Accepted-&gt;Manually Rejected)</t>
+  </si>
+  <si>
+    <t>Preparing ppt for PT ; Discussion on normal trade flow test cases; Discussion on rectified trade flow with nirajan; Dicussion on settlement module</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,6 +498,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -555,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -667,6 +680,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6168,8 +6184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -7497,7 +7513,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7743,7 +7761,9 @@
       <c r="F11" s="38">
         <v>0.75</v>
       </c>
-      <c r="G11" s="41"/>
+      <c r="G11" s="43" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="35">
@@ -7764,7 +7784,9 @@
       <c r="F12" s="38">
         <v>0.75</v>
       </c>
-      <c r="G12" s="42"/>
+      <c r="G12" s="42" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="35">
@@ -7810,6 +7832,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>